<commit_message>
added different os functionality
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -437,22 +437,22 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Tempo</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Genre</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Artist Name</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Track Name</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Genre</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Tempo</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Artist Name</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">

</xml_diff>